<commit_message>
updated correctionfactors.csv for Fuel cell engines and related functions in energy.py
</commit_message>
<xml_diff>
--- a/notebooks/Correctionfactors.xlsx
+++ b/notebooks/Correctionfactors.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loes\Documents\Afstuderen\Python\Data bestandjes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manjiang\OpenTNSim\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F2513CF-3FBE-4A13-A4AB-336908CF34A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80E930A9-DECA-419C-BB0C-EE7A8BF1AFB6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>% Partial engine load</t>
   </si>
@@ -55,11 +54,17 @@
   <si>
     <t>Nox IWP/IWA-v/c-4</t>
   </si>
+  <si>
+    <t>renewable energy sources in SOFC Fuel cell engine</t>
+  </si>
+  <si>
+    <t>renewable energy sources in PEMFC Fuel cell engine</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -113,9 +118,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -128,6 +139,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>61652</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>537653</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7023100" y="1820602"/>
+          <a:ext cx="5065203" cy="2329619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,19 +480,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38850C12-EB10-4A02-A587-635355F04209}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.36328125" customWidth="1"/>
+    <col min="2" max="5" width="24.36328125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="9" width="26.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +519,14 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>0.05</v>
       </c>
@@ -483,8 +548,14 @@
       <c r="G2" s="4">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H2" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>0.1</v>
       </c>
@@ -506,8 +577,14 @@
       <c r="G3" s="4">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H3" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>0.15</v>
       </c>
@@ -529,8 +606,14 @@
       <c r="G4" s="4">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>0.2</v>
       </c>
@@ -552,8 +635,14 @@
       <c r="G5" s="4">
         <v>1.19</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>0.25</v>
       </c>
@@ -575,8 +664,14 @@
       <c r="G6" s="4">
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>0.3</v>
       </c>
@@ -598,8 +693,14 @@
       <c r="G7" s="4">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H7" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>0.35</v>
       </c>
@@ -621,8 +722,14 @@
       <c r="G8" s="4">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H8" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>0.4</v>
       </c>
@@ -644,8 +751,14 @@
       <c r="G9" s="4">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H9" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>0.45</v>
       </c>
@@ -667,8 +780,14 @@
       <c r="G10" s="4">
         <v>1.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H10" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>0.5</v>
       </c>
@@ -690,8 +809,14 @@
       <c r="G11" s="4">
         <v>1.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H11" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>0.55000000000000004</v>
       </c>
@@ -713,8 +838,14 @@
       <c r="G12" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H12" s="7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>0.6</v>
       </c>
@@ -736,8 +867,14 @@
       <c r="G13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H13" s="7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>0.65</v>
       </c>
@@ -759,8 +896,14 @@
       <c r="G14" s="4">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H14" s="7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>0.7</v>
       </c>
@@ -782,8 +925,14 @@
       <c r="G15" s="4">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H15" s="7">
+        <v>1.19</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>0.75</v>
       </c>
@@ -805,8 +954,14 @@
       <c r="G16" s="4">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H16" s="7">
+        <v>1.19</v>
+      </c>
+      <c r="I16" s="7">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>0.8</v>
       </c>
@@ -828,8 +983,14 @@
       <c r="G17" s="4">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H17" s="7">
+        <v>1.19</v>
+      </c>
+      <c r="I17" s="7">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>0.85</v>
       </c>
@@ -851,8 +1012,14 @@
       <c r="G18" s="4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H18" s="7">
+        <v>1.19</v>
+      </c>
+      <c r="I18" s="7">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>0.9</v>
       </c>
@@ -874,8 +1041,14 @@
       <c r="G19" s="4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H19" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>0.95</v>
       </c>
@@ -897,8 +1070,14 @@
       <c r="G20" s="4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="H20" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -920,8 +1099,14 @@
       <c r="G21" s="4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="I21" s="7">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -930,7 +1115,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -941,5 +1126,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validation example and renewable in Rhine ARA
</commit_message>
<xml_diff>
--- a/notebooks/Correctionfactors.xlsx
+++ b/notebooks/Correctionfactors.xlsx
@@ -483,14 +483,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" customWidth="1"/>
-    <col min="2" max="5" width="24.36328125" hidden="1" customWidth="1"/>
+    <col min="1" max="4" width="24.36328125" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" customWidth="1"/>
     <col min="8" max="8" width="30.7265625" customWidth="1"/>

</xml_diff>